<commit_message>
modified:   W04_218518_2019_praca magisterska.docx 	modified:   obrazy/panorama.jpg 	modified:   wyniki.xlsx
</commit_message>
<xml_diff>
--- a/wyniki.xlsx
+++ b/wyniki.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Clouds\OneDrive\Polibuda\Praca magisterska\1. Praca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9D2646-A7BD-44E8-9D79-DEE0CA86A1F2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A6D8C3-F476-4D9A-B79D-8E4E4988D1EE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C12735B6-8E7C-4A52-A671-96CF398497BB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{C12735B6-8E7C-4A52-A671-96CF398497BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -841,7 +841,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Procent nieznalezionych regionów</a:t>
+              <a:t>Procent błędnie znalezionych regionów</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -7847,12 +7847,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F01B856-5989-43A7-867A-97FA0332578A}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="Z16" sqref="Z16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="10" max="13" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
modified:   W04_218518_2019_praca magisterska.docx 	modified:   wyniki.xlsx
</commit_message>
<xml_diff>
--- a/wyniki.xlsx
+++ b/wyniki.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Clouds\OneDrive\Polibuda\Praca magisterska\1. Praca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A6D8C3-F476-4D9A-B79D-8E4E4988D1EE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="6_{970B4553-086E-41DC-B42A-43C0B080C0CB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{96ECA135-35A4-48FE-A29E-0010E5435A84}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{C12735B6-8E7C-4A52-A671-96CF398497BB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C12735B6-8E7C-4A52-A671-96CF398497BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -2855,30 +2855,30 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>(Arkusz1!$C$6,Arkusz1!$C$15,Arkusz1!$C$24,Arkusz1!$C$33,Arkusz1!$C$42,Arkusz1!$C$51,Arkusz1!$C$60)</c:f>
+              <c:f>(Arkusz1!$C$7,Arkusz1!$C$16,Arkusz1!$C$25,Arkusz1!$C$34,Arkusz1!$C$43,Arkusz1!$C$52,Arkusz1!$C$61)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>22.22</c:v>
+                  <c:v>14.63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.02</c:v>
+                  <c:v>12.82</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.57</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.8</c:v>
+                  <c:v>13.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22.95</c:v>
+                  <c:v>14.28</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.510000000000002</c:v>
+                  <c:v>12.76</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20.37</c:v>
+                  <c:v>13.63</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2907,30 +2907,30 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>(Arkusz1!$D$6,Arkusz1!$D$15,Arkusz1!$D$24,Arkusz1!$D$33,Arkusz1!$D$42,Arkusz1!$D$51,Arkusz1!$D$60)</c:f>
+              <c:f>(Arkusz1!$D$7,Arkusz1!$D$16,Arkusz1!$D$25,Arkusz1!$D$34,Arkusz1!$D$43,Arkusz1!$D$52,Arkusz1!$D$61)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>28.57</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.76</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33.33</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33.33</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2949,7 +2949,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4"/>
+              <a:srgbClr val="FFC000"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -2959,27 +2959,27 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>(Arkusz1!$E$6,Arkusz1!$E$15,Arkusz1!$E$24,Arkusz1!$E$33,Arkusz1!$E$42,Arkusz1!$E$51,Arkusz1!$E$61)</c:f>
+              <c:f>(Arkusz1!$E$7,Arkusz1!$E$16,Arkusz1!$E$25,Arkusz1!$E$34,Arkusz1!$E$43,Arkusz1!$E$52,Arkusz1!$E$61)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>29.41</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27.77</c:v>
+                  <c:v>66.66</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60</c:v>
+                  <c:v>22.22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28.57</c:v>
+                  <c:v>71.150000000000006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.36</c:v>
+                  <c:v>53.48</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34.78</c:v>
+                  <c:v>48.88</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>58.57</c:v>
@@ -3040,30 +3040,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Arkusz1!$F$6,Arkusz1!$F$15,Arkusz1!$F$24,Arkusz1!$F$33,Arkusz1!$F$42,Arkusz1!$F$51,Arkusz1!$F$60)</c:f>
+              <c:f>(Arkusz1!$F$7,Arkusz1!$F$16,Arkusz1!$F$25,Arkusz1!$F$34,Arkusz1!$F$43,Arkusz1!$F$52,Arkusz1!$F$61)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>24.35</c:v>
+                  <c:v>37.869999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.42</c:v>
+                  <c:v>33.33</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41.66</c:v>
+                  <c:v>17.850000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.97</c:v>
+                  <c:v>35.549999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26.66</c:v>
+                  <c:v>31.91</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.39</c:v>
+                  <c:v>28.86</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24.37</c:v>
+                  <c:v>32.51</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7848,7 +7848,7 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8975,8 +8975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E1B7D-4C2A-4D5B-ADF2-162B8355AEC4}">
   <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>